<commit_message>
[FIX] import journal in asset
</commit_message>
<xml_diff>
--- a/pabi_import_journal_entries/xlsx_template/import_journal_entries.xlsx
+++ b/pabi_import_journal_entries/xlsx_template/import_journal_entries.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t xml:space="preserve">Import Journal Entries</t>
   </si>
@@ -76,6 +76,15 @@
     <t xml:space="preserve">Activity</t>
   </si>
   <si>
+    <t xml:space="preserve">Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Profile Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">REF1</t>
   </si>
   <si>
@@ -88,6 +97,12 @@
     <t xml:space="preserve">aaa</t>
   </si>
   <si>
+    <t xml:space="preserve">6115-001-0001 - เครื่องกำเนิดไฟฟ้าแผงและชนิดต่างๆ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9990-001-0001-000001227</t>
+  </si>
+  <si>
     <t xml:space="preserve">PO1002</t>
   </si>
   <si>
@@ -101,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">ccc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9200-001-0001-000005376</t>
   </si>
   <si>
     <t xml:space="preserve">PO1004</t>
@@ -168,7 +186,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,7 +196,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD4D1"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFF7D1D5"/>
       </patternFill>
     </fill>
     <fill>
@@ -197,6 +215,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFADD58A"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D1D5"/>
+        <bgColor rgb="FFFCD4D1"/>
       </patternFill>
     </fill>
   </fills>
@@ -249,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,6 +330,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -320,12 +348,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -352,7 +380,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -401,7 +429,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
@@ -409,17 +437,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="17" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -454,7 +484,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -502,6 +532,15 @@
       </c>
       <c r="P2" s="13" t="s">
         <v>17</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
@@ -511,11 +550,11 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>19</v>
+      <c r="A3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>43393</v>
@@ -527,10 +566,10 @@
         <v>1210010001</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>10000</v>
@@ -538,15 +577,21 @@
       <c r="K3" s="0" t="n">
         <v>101009</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>19</v>
+    <row r="4" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>43393</v>
@@ -555,25 +600,29 @@
       <c r="E4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="15" t="n">
+      <c r="F4" s="16" t="n">
         <v>1210010001</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>22</v>
+      <c r="G4" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="K4" s="15" t="n">
+      <c r="K4" s="16" t="n">
         <v>101009</v>
       </c>
       <c r="N4" s="0"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="0"/>
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
       <c r="AMG4" s="0"/>
@@ -582,11 +631,11 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>19</v>
+      <c r="A5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>43393</v>
@@ -598,10 +647,10 @@
         <v>1210010001</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>10000</v>
@@ -609,15 +658,21 @@
       <c r="K5" s="0" t="n">
         <v>101009</v>
       </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>19</v>
+    <row r="6" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>43393</v>
@@ -626,25 +681,28 @@
       <c r="E6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="15" t="n">
+      <c r="F6" s="16" t="n">
         <v>1210010001</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>27</v>
+      <c r="G6" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="K6" s="15" t="n">
+      <c r="K6" s="16" t="n">
         <v>101009</v>
       </c>
       <c r="N6" s="0"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="AME6" s="0"/>
       <c r="AMF6" s="0"/>
       <c r="AMG6" s="0"/>

</xml_diff>

<commit_message>
[FIX] delete asset profile code not import
</commit_message>
<xml_diff>
--- a/pabi_import_journal_entries/xlsx_template/import_journal_entries.xlsx
+++ b/pabi_import_journal_entries/xlsx_template/import_journal_entries.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t xml:space="preserve">Import Journal Entries</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Asset Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Profile Code</t>
   </si>
   <si>
     <t xml:space="preserve">REF1</t>
@@ -429,7 +426,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.73"/>
@@ -477,6 +474,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
+      <c r="S1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -539,9 +537,7 @@
       <c r="R2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="S2" s="0"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
@@ -551,10 +547,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>43393</v>
@@ -566,10 +562,10 @@
         <v>1210010001</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>10000</v>
@@ -580,18 +576,18 @@
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>43393</v>
@@ -604,10 +600,10 @@
         <v>1210010001</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="n">
@@ -620,9 +616,10 @@
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
       <c r="Q4" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
       <c r="AMG4" s="0"/>
@@ -632,10 +629,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>43393</v>
@@ -647,10 +644,10 @@
         <v>1210010001</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>10000</v>
@@ -661,18 +658,18 @@
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>43393</v>
@@ -685,10 +682,10 @@
         <v>1210010001</v>
       </c>
       <c r="G6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="n">
@@ -701,8 +698,9 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="S6" s="0"/>
       <c r="AME6" s="0"/>
       <c r="AMF6" s="0"/>
       <c r="AMG6" s="0"/>

</xml_diff>